<commit_message>
feat: checked server usability
1. download can be performed in different platform
2. details of student added to correction page
3. download button is added
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:EM1"/>
+  <dimension ref="A1:EM5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,7 @@
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>攏(lóng)</t>
+          <t>攏(lóng) 造句</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
@@ -516,7 +516,7 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>到(kàu)</t>
+          <t>到(kàu) 造句</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
-          <t>阿媽(a-má)</t>
+          <t>阿媽(a-má) 造句</t>
         </is>
       </c>
       <c r="T1" s="1" t="inlineStr">
@@ -536,7 +536,7 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>兜(tau)</t>
+          <t>兜(tau) 造句</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
@@ -546,7 +546,7 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>和(hām)</t>
+          <t>和(hām) 造句</t>
         </is>
       </c>
       <c r="X1" s="1" t="inlineStr">
@@ -556,7 +556,7 @@
       </c>
       <c r="Y1" s="1" t="inlineStr">
         <is>
-          <t>故事(kòo-sū)</t>
+          <t>故事(kòo-sū) 造句</t>
         </is>
       </c>
       <c r="Z1" s="1" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="AA1" s="1" t="inlineStr">
         <is>
-          <t>煩惱(huân-ló)</t>
+          <t>煩惱(huân-ló) 造句</t>
         </is>
       </c>
       <c r="AB1" s="1" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="AC1" s="1" t="inlineStr">
         <is>
-          <t>趕緊(kuánn-kín)</t>
+          <t>趕緊(kuánn-kín) 造句</t>
         </is>
       </c>
       <c r="AD1" s="1" t="inlineStr">
@@ -586,7 +586,7 @@
       </c>
       <c r="AE1" s="1" t="inlineStr">
         <is>
-          <t>歇睏(hioh-khùn)</t>
+          <t>歇睏(hioh-khùn) 造句</t>
         </is>
       </c>
       <c r="AF1" s="1" t="inlineStr">
@@ -596,7 +596,7 @@
       </c>
       <c r="AG1" s="1" t="inlineStr">
         <is>
-          <t>目屎(ba̍k-sái)</t>
+          <t>目屎(ba̍k-sái) 造句</t>
         </is>
       </c>
       <c r="AH1" s="1" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="AI1" s="1" t="inlineStr">
         <is>
-          <t>少年(siàu-liân)</t>
+          <t>少年(siàu-liân) 造句</t>
         </is>
       </c>
       <c r="AJ1" s="1" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="AK1" s="1" t="inlineStr">
         <is>
-          <t>後壁(āu-piah)</t>
+          <t>後壁(āu-piah) 造句</t>
         </is>
       </c>
       <c r="AL1" s="1" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="AM1" s="1" t="inlineStr">
         <is>
-          <t>呵咾(o-ló)</t>
+          <t>呵咾(o-ló) 造句</t>
         </is>
       </c>
       <c r="AN1" s="1" t="inlineStr">
@@ -636,7 +636,7 @@
       </c>
       <c r="AO1" s="1" t="inlineStr">
         <is>
-          <t>分鐘(hun-tsing)</t>
+          <t>分鐘(hun-tsing) 造句</t>
         </is>
       </c>
       <c r="AP1" s="1" t="inlineStr">
@@ -646,7 +646,7 @@
       </c>
       <c r="AQ1" s="1" t="inlineStr">
         <is>
-          <t>清氣(tshing-khì)</t>
+          <t>清氣(tshing-khì) 造句</t>
         </is>
       </c>
       <c r="AR1" s="1" t="inlineStr">
@@ -656,7 +656,7 @@
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>小等(sió-tán)</t>
+          <t>小等(sió-tán) 造句</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
@@ -666,7 +666,7 @@
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>天氣(thinn-khì)</t>
+          <t>天氣(thinn-khì) 造句</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="AW1" s="1" t="inlineStr">
         <is>
-          <t>低(kē)</t>
+          <t>低(kē) 造句</t>
         </is>
       </c>
       <c r="AX1" s="1" t="inlineStr">
@@ -686,7 +686,7 @@
       </c>
       <c r="AY1" s="1" t="inlineStr">
         <is>
-          <t>好耍(hó-sńg)</t>
+          <t>好耍(hó-sńg) 造句</t>
         </is>
       </c>
       <c r="AZ1" s="1" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="BA1" s="1" t="inlineStr">
         <is>
-          <t>亂(luān)</t>
+          <t>亂(luān) 造句</t>
         </is>
       </c>
       <c r="BB1" s="1" t="inlineStr">
@@ -706,7 +706,7 @@
       </c>
       <c r="BC1" s="1" t="inlineStr">
         <is>
-          <t>新聞(sin-bûn)</t>
+          <t>新聞(sin-bûn) 造句</t>
         </is>
       </c>
       <c r="BD1" s="1" t="inlineStr">
@@ -716,7 +716,7 @@
       </c>
       <c r="BE1" s="1" t="inlineStr">
         <is>
-          <t>地球(tē-kiû)</t>
+          <t>地球(tē-kiû) 造句</t>
         </is>
       </c>
       <c r="BF1" s="1" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="BG1" s="1" t="inlineStr">
         <is>
-          <t>記(kì)</t>
+          <t>記(kì) 造句</t>
         </is>
       </c>
       <c r="BH1" s="1" t="inlineStr">
@@ -736,7 +736,7 @@
       </c>
       <c r="BI1" s="1" t="inlineStr">
         <is>
-          <t>拭(tshit)</t>
+          <t>拭(tshit) 造句</t>
         </is>
       </c>
       <c r="BJ1" s="1" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="BK1" s="1" t="inlineStr">
         <is>
-          <t>溫暖(un-luán)</t>
+          <t>溫暖(un-luán) 造句</t>
         </is>
       </c>
       <c r="BL1" s="1" t="inlineStr">
@@ -756,7 +756,7 @@
       </c>
       <c r="BM1" s="1" t="inlineStr">
         <is>
-          <t>保持(pó-tshî)</t>
+          <t>保持(pó-tshî) 造句</t>
         </is>
       </c>
       <c r="BN1" s="1" t="inlineStr">
@@ -766,7 +766,7 @@
       </c>
       <c r="BO1" s="1" t="inlineStr">
         <is>
-          <t>回答(huê-tap)</t>
+          <t>回答(huê-tap) 造句</t>
         </is>
       </c>
       <c r="BP1" s="1" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="BQ1" s="1" t="inlineStr">
         <is>
-          <t>詳細(siông-sè)</t>
+          <t>詳細(siông-sè) 造句</t>
         </is>
       </c>
       <c r="BR1" s="1" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="BS1" s="1" t="inlineStr">
         <is>
-          <t>所費(sóo-huì)</t>
+          <t>所費(sóo-huì) 造句</t>
         </is>
       </c>
       <c r="BT1" s="1" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="BU1" s="1" t="inlineStr">
         <is>
-          <t>開喙(khui-tshuì)</t>
+          <t>開喙(khui-tshuì) 造句</t>
         </is>
       </c>
       <c r="BV1" s="1" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="BW1" s="1" t="inlineStr">
         <is>
-          <t>切(tshiat)</t>
+          <t>切(tshiat) 造句</t>
         </is>
       </c>
       <c r="BX1" s="1" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="BY1" s="1" t="inlineStr">
         <is>
-          <t>抹(buah)</t>
+          <t>抹(buah) 造句</t>
         </is>
       </c>
       <c r="BZ1" s="1" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="CA1" s="1" t="inlineStr">
         <is>
-          <t>巡(sûn)</t>
+          <t>巡(sûn) 造句</t>
         </is>
       </c>
       <c r="CB1" s="1" t="inlineStr">
@@ -836,7 +836,7 @@
       </c>
       <c r="CC1" s="1" t="inlineStr">
         <is>
-          <t>體會(thé-huē)</t>
+          <t>體會(thé-huē) 造句</t>
         </is>
       </c>
       <c r="CD1" s="1" t="inlineStr">
@@ -846,7 +846,7 @@
       </c>
       <c r="CE1" s="1" t="inlineStr">
         <is>
-          <t>天公伯仔(thinn-kong-peh-á)</t>
+          <t>天公伯仔(thinn-kong-peh-á) 造句</t>
         </is>
       </c>
       <c r="CF1" s="1" t="inlineStr">
@@ -856,7 +856,7 @@
       </c>
       <c r="CG1" s="1" t="inlineStr">
         <is>
-          <t>雞卵糕(ke-nn̄g-ko)</t>
+          <t>雞卵糕(ke-nn̄g-ko) 造句</t>
         </is>
       </c>
       <c r="CH1" s="1" t="inlineStr">
@@ -866,7 +866,7 @@
       </c>
       <c r="CI1" s="1" t="inlineStr">
         <is>
-          <t>炊(tshue)</t>
+          <t>炊(tshue) 造句</t>
         </is>
       </c>
       <c r="CJ1" s="1" t="inlineStr">
@@ -876,7 +876,7 @@
       </c>
       <c r="CK1" s="1" t="inlineStr">
         <is>
-          <t>主任(tsú-jīm)</t>
+          <t>主任(tsú-jīm) 造句</t>
         </is>
       </c>
       <c r="CL1" s="1" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="CM1" s="1" t="inlineStr">
         <is>
-          <t>速度(sok-tōo)</t>
+          <t>速度(sok-tōo) 造句</t>
         </is>
       </c>
       <c r="CN1" s="1" t="inlineStr">
@@ -896,7 +896,7 @@
       </c>
       <c r="CO1" s="1" t="inlineStr">
         <is>
-          <t>生理人(sing-lí-lâng)</t>
+          <t>生理人(sing-lí-lâng) 造句</t>
         </is>
       </c>
       <c r="CP1" s="1" t="inlineStr">
@@ -906,7 +906,7 @@
       </c>
       <c r="CQ1" s="1" t="inlineStr">
         <is>
-          <t>鼓(kóo)</t>
+          <t>鼓(kóo) 造句</t>
         </is>
       </c>
       <c r="CR1" s="1" t="inlineStr">
@@ -916,7 +916,7 @@
       </c>
       <c r="CS1" s="1" t="inlineStr">
         <is>
-          <t>國際(kok-tsè)</t>
+          <t>國際(kok-tsè) 造句</t>
         </is>
       </c>
       <c r="CT1" s="1" t="inlineStr">
@@ -926,7 +926,7 @@
       </c>
       <c r="CU1" s="1" t="inlineStr">
         <is>
-          <t>古蹟(kóo-tsik)</t>
+          <t>古蹟(kóo-tsik) 造句</t>
         </is>
       </c>
       <c r="CV1" s="1" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
       <c r="CW1" s="1" t="inlineStr">
         <is>
-          <t>頂真(tíng-tsin)</t>
+          <t>頂真(tíng-tsin) 造句</t>
         </is>
       </c>
       <c r="CX1" s="1" t="inlineStr">
@@ -946,7 +946,7 @@
       </c>
       <c r="CY1" s="1" t="inlineStr">
         <is>
-          <t>外面(guā-bīn)</t>
+          <t>外面(guā-bīn) 造句</t>
         </is>
       </c>
       <c r="CZ1" s="1" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="DA1" s="1" t="inlineStr">
         <is>
-          <t>蝶仔(ia̍h-á)</t>
+          <t>蝶仔(ia̍h-á) 造句</t>
         </is>
       </c>
       <c r="DB1" s="1" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="DC1" s="1" t="inlineStr">
         <is>
-          <t>事實(sū-si̍t)</t>
+          <t>事實(sū-si̍t) 造句</t>
         </is>
       </c>
       <c r="DD1" s="1" t="inlineStr">
@@ -976,7 +976,7 @@
       </c>
       <c r="DE1" s="1" t="inlineStr">
         <is>
-          <t>鬧熱滾滾(lāu-jia̍t-kún-kún)</t>
+          <t>鬧熱滾滾(lāu-jia̍t-kún-kún) 造句</t>
         </is>
       </c>
       <c r="DF1" s="1" t="inlineStr">
@@ -986,7 +986,7 @@
       </c>
       <c r="DG1" s="1" t="inlineStr">
         <is>
-          <t>圓箍仔(înn-khoo-á)</t>
+          <t>圓箍仔(înn-khoo-á) 造句</t>
         </is>
       </c>
       <c r="DH1" s="1" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="DI1" s="1" t="inlineStr">
         <is>
-          <t>隊(tuī)</t>
+          <t>隊(tuī) 造句</t>
         </is>
       </c>
       <c r="DJ1" s="1" t="inlineStr">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="DK1" s="1" t="inlineStr">
         <is>
-          <t>郵票(iû-phiò)</t>
+          <t>郵票(iû-phiò) 造句</t>
         </is>
       </c>
       <c r="DL1" s="1" t="inlineStr">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="DM1" s="1" t="inlineStr">
         <is>
-          <t>手套(tshiú-thò)</t>
+          <t>手套(tshiú-thò) 造句</t>
         </is>
       </c>
       <c r="DN1" s="1" t="inlineStr">
@@ -1026,7 +1026,7 @@
       </c>
       <c r="DO1" s="1" t="inlineStr">
         <is>
-          <t>做法(tsò-huat)</t>
+          <t>做法(tsò-huat) 造句</t>
         </is>
       </c>
       <c r="DP1" s="1" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="DQ1" s="1" t="inlineStr">
         <is>
-          <t>性地(sìng-tē)</t>
+          <t>性地(sìng-tē) 造句</t>
         </is>
       </c>
       <c r="DR1" s="1" t="inlineStr">
@@ -1046,7 +1046,7 @@
       </c>
       <c r="DS1" s="1" t="inlineStr">
         <is>
-          <t>蓮霧(lián-bū)</t>
+          <t>蓮霧(lián-bū) 造句</t>
         </is>
       </c>
       <c r="DT1" s="1" t="inlineStr">
@@ -1056,7 +1056,7 @@
       </c>
       <c r="DU1" s="1" t="inlineStr">
         <is>
-          <t>本錢(pún-tsînn)</t>
+          <t>本錢(pún-tsînn) 造句</t>
         </is>
       </c>
       <c r="DV1" s="1" t="inlineStr">
@@ -1066,7 +1066,7 @@
       </c>
       <c r="DW1" s="1" t="inlineStr">
         <is>
-          <t>水桶(tsuí-tháng)</t>
+          <t>水桶(tsuí-tháng) 造句</t>
         </is>
       </c>
       <c r="DX1" s="1" t="inlineStr">
@@ -1076,7 +1076,7 @@
       </c>
       <c r="DY1" s="1" t="inlineStr">
         <is>
-          <t>運動會(ūn-tōng-huē)</t>
+          <t>運動會(ūn-tōng-huē) 造句</t>
         </is>
       </c>
       <c r="DZ1" s="1" t="inlineStr">
@@ -1086,7 +1086,7 @@
       </c>
       <c r="EA1" s="1" t="inlineStr">
         <is>
-          <t>落雪(lo̍h-seh)</t>
+          <t>落雪(lo̍h-seh) 造句</t>
         </is>
       </c>
       <c r="EB1" s="1" t="inlineStr">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="EC1" s="1" t="inlineStr">
         <is>
-          <t>源頭(guân-thâu)</t>
+          <t>源頭(guân-thâu) 造句</t>
         </is>
       </c>
       <c r="ED1" s="1" t="inlineStr">
@@ -1106,7 +1106,7 @@
       </c>
       <c r="EE1" s="1" t="inlineStr">
         <is>
-          <t>萬事(bān-sū)</t>
+          <t>萬事(bān-sū) 造句</t>
         </is>
       </c>
       <c r="EF1" s="1" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="EG1" s="1" t="inlineStr">
         <is>
-          <t>著驚(tio̍h-kiann)</t>
+          <t>著驚(tio̍h-kiann) 造句</t>
         </is>
       </c>
       <c r="EH1" s="1" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="EI1" s="1" t="inlineStr">
         <is>
-          <t>烏青(oo-tshenn)</t>
+          <t>烏青(oo-tshenn) 造句</t>
         </is>
       </c>
       <c r="EJ1" s="1" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="EK1" s="1" t="inlineStr">
         <is>
-          <t>羅馬字(lô-má-jī)</t>
+          <t>羅馬字(lô-má-jī) 造句</t>
         </is>
       </c>
       <c r="EL1" s="1" t="inlineStr">
@@ -1146,9 +1146,717 @@
       </c>
       <c r="EM1" s="1" t="inlineStr">
         <is>
-          <t>報應(pò-ìng)</t>
-        </is>
-      </c>
+          <t>報應(pò-ìng) 造句</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>市立將軍國小114693</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>翁麒倫</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
+      <c r="AB2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr"/>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
+      <c r="AR2" t="inlineStr"/>
+      <c r="AS2" t="inlineStr"/>
+      <c r="AT2" t="inlineStr"/>
+      <c r="AU2" t="inlineStr"/>
+      <c r="AV2" t="inlineStr"/>
+      <c r="AW2" t="inlineStr"/>
+      <c r="AX2" t="inlineStr"/>
+      <c r="AY2" t="inlineStr"/>
+      <c r="AZ2" t="inlineStr"/>
+      <c r="BA2" t="inlineStr"/>
+      <c r="BB2" t="inlineStr"/>
+      <c r="BC2" t="inlineStr"/>
+      <c r="BD2" t="inlineStr"/>
+      <c r="BE2" t="inlineStr"/>
+      <c r="BF2" t="inlineStr"/>
+      <c r="BG2" t="inlineStr"/>
+      <c r="BH2" t="inlineStr"/>
+      <c r="BI2" t="inlineStr"/>
+      <c r="BJ2" t="inlineStr"/>
+      <c r="BK2" t="inlineStr"/>
+      <c r="BL2" t="inlineStr"/>
+      <c r="BM2" t="inlineStr"/>
+      <c r="BN2" t="inlineStr"/>
+      <c r="BO2" t="inlineStr"/>
+      <c r="BP2" t="inlineStr"/>
+      <c r="BQ2" t="inlineStr"/>
+      <c r="BR2" t="inlineStr"/>
+      <c r="BS2" t="inlineStr"/>
+      <c r="BT2" t="inlineStr"/>
+      <c r="BU2" t="inlineStr"/>
+      <c r="BV2" t="inlineStr"/>
+      <c r="BW2" t="inlineStr"/>
+      <c r="BX2" t="inlineStr"/>
+      <c r="BY2" t="inlineStr"/>
+      <c r="BZ2" t="inlineStr"/>
+      <c r="CA2" t="inlineStr"/>
+      <c r="CB2" t="inlineStr"/>
+      <c r="CC2" t="inlineStr"/>
+      <c r="CD2" t="inlineStr"/>
+      <c r="CE2" t="inlineStr"/>
+      <c r="CF2" t="inlineStr"/>
+      <c r="CG2" t="inlineStr"/>
+      <c r="CH2" t="inlineStr"/>
+      <c r="CI2" t="inlineStr"/>
+      <c r="CJ2" t="inlineStr"/>
+      <c r="CK2" t="inlineStr"/>
+      <c r="CL2" t="inlineStr"/>
+      <c r="CM2" t="inlineStr"/>
+      <c r="CN2" t="inlineStr"/>
+      <c r="CO2" t="inlineStr"/>
+      <c r="CP2" t="inlineStr"/>
+      <c r="CQ2" t="inlineStr"/>
+      <c r="CR2" t="inlineStr"/>
+      <c r="CS2" t="inlineStr"/>
+      <c r="CT2" t="inlineStr"/>
+      <c r="CU2" t="inlineStr"/>
+      <c r="CV2" t="inlineStr"/>
+      <c r="CW2" t="inlineStr"/>
+      <c r="CX2" t="inlineStr"/>
+      <c r="CY2" t="inlineStr"/>
+      <c r="CZ2" t="inlineStr"/>
+      <c r="DA2" t="inlineStr"/>
+      <c r="DB2" t="inlineStr"/>
+      <c r="DC2" t="inlineStr"/>
+      <c r="DD2" t="inlineStr"/>
+      <c r="DE2" t="inlineStr"/>
+      <c r="DF2" t="inlineStr"/>
+      <c r="DG2" t="inlineStr"/>
+      <c r="DH2" t="inlineStr"/>
+      <c r="DI2" t="inlineStr"/>
+      <c r="DJ2" t="inlineStr"/>
+      <c r="DK2" t="inlineStr"/>
+      <c r="DL2" t="inlineStr"/>
+      <c r="DM2" t="inlineStr"/>
+      <c r="DN2" t="inlineStr"/>
+      <c r="DO2" t="inlineStr"/>
+      <c r="DP2" t="inlineStr"/>
+      <c r="DQ2" t="inlineStr"/>
+      <c r="DR2" t="inlineStr"/>
+      <c r="DS2" t="inlineStr"/>
+      <c r="DT2" t="inlineStr"/>
+      <c r="DU2" t="inlineStr"/>
+      <c r="DV2" t="inlineStr"/>
+      <c r="DW2" t="inlineStr"/>
+      <c r="DX2" t="inlineStr"/>
+      <c r="DY2" t="inlineStr"/>
+      <c r="DZ2" t="inlineStr"/>
+      <c r="EA2" t="inlineStr"/>
+      <c r="EB2" t="inlineStr"/>
+      <c r="EC2" t="inlineStr"/>
+      <c r="ED2" t="inlineStr"/>
+      <c r="EE2" t="inlineStr"/>
+      <c r="EF2" t="inlineStr"/>
+      <c r="EG2" t="inlineStr"/>
+      <c r="EH2" t="inlineStr"/>
+      <c r="EI2" t="inlineStr"/>
+      <c r="EJ2" t="inlineStr"/>
+      <c r="EK2" t="inlineStr"/>
+      <c r="EL2" t="inlineStr"/>
+      <c r="EM2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>市立將軍國小114693</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>吳姿穎</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="n">
+        <v>1</v>
+      </c>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="inlineStr"/>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
+      <c r="AR3" t="inlineStr"/>
+      <c r="AS3" t="inlineStr"/>
+      <c r="AT3" t="inlineStr"/>
+      <c r="AU3" t="inlineStr"/>
+      <c r="AV3" t="inlineStr"/>
+      <c r="AW3" t="inlineStr"/>
+      <c r="AX3" t="inlineStr"/>
+      <c r="AY3" t="inlineStr"/>
+      <c r="AZ3" t="inlineStr"/>
+      <c r="BA3" t="inlineStr"/>
+      <c r="BB3" t="inlineStr"/>
+      <c r="BC3" t="inlineStr"/>
+      <c r="BD3" t="inlineStr"/>
+      <c r="BE3" t="inlineStr"/>
+      <c r="BF3" t="inlineStr"/>
+      <c r="BG3" t="inlineStr"/>
+      <c r="BH3" t="inlineStr"/>
+      <c r="BI3" t="inlineStr"/>
+      <c r="BJ3" t="inlineStr"/>
+      <c r="BK3" t="inlineStr"/>
+      <c r="BL3" t="inlineStr"/>
+      <c r="BM3" t="inlineStr"/>
+      <c r="BN3" t="inlineStr"/>
+      <c r="BO3" t="inlineStr"/>
+      <c r="BP3" t="inlineStr"/>
+      <c r="BQ3" t="inlineStr"/>
+      <c r="BR3" t="inlineStr"/>
+      <c r="BS3" t="inlineStr"/>
+      <c r="BT3" t="inlineStr"/>
+      <c r="BU3" t="inlineStr"/>
+      <c r="BV3" t="inlineStr"/>
+      <c r="BW3" t="inlineStr"/>
+      <c r="BX3" t="inlineStr"/>
+      <c r="BY3" t="inlineStr"/>
+      <c r="BZ3" t="inlineStr"/>
+      <c r="CA3" t="inlineStr"/>
+      <c r="CB3" t="inlineStr"/>
+      <c r="CC3" t="inlineStr"/>
+      <c r="CD3" t="inlineStr"/>
+      <c r="CE3" t="inlineStr"/>
+      <c r="CF3" t="inlineStr"/>
+      <c r="CG3" t="inlineStr"/>
+      <c r="CH3" t="inlineStr"/>
+      <c r="CI3" t="inlineStr"/>
+      <c r="CJ3" t="inlineStr"/>
+      <c r="CK3" t="inlineStr"/>
+      <c r="CL3" t="inlineStr"/>
+      <c r="CM3" t="inlineStr"/>
+      <c r="CN3" t="inlineStr"/>
+      <c r="CO3" t="inlineStr"/>
+      <c r="CP3" t="inlineStr"/>
+      <c r="CQ3" t="inlineStr"/>
+      <c r="CR3" t="inlineStr"/>
+      <c r="CS3" t="inlineStr"/>
+      <c r="CT3" t="inlineStr"/>
+      <c r="CU3" t="inlineStr"/>
+      <c r="CV3" t="inlineStr"/>
+      <c r="CW3" t="inlineStr"/>
+      <c r="CX3" t="inlineStr"/>
+      <c r="CY3" t="inlineStr"/>
+      <c r="CZ3" t="inlineStr"/>
+      <c r="DA3" t="inlineStr"/>
+      <c r="DB3" t="inlineStr"/>
+      <c r="DC3" t="inlineStr"/>
+      <c r="DD3" t="inlineStr"/>
+      <c r="DE3" t="inlineStr"/>
+      <c r="DF3" t="inlineStr"/>
+      <c r="DG3" t="inlineStr"/>
+      <c r="DH3" t="inlineStr"/>
+      <c r="DI3" t="inlineStr"/>
+      <c r="DJ3" t="inlineStr"/>
+      <c r="DK3" t="inlineStr"/>
+      <c r="DL3" t="inlineStr"/>
+      <c r="DM3" t="inlineStr"/>
+      <c r="DN3" t="inlineStr"/>
+      <c r="DO3" t="inlineStr"/>
+      <c r="DP3" t="inlineStr"/>
+      <c r="DQ3" t="inlineStr"/>
+      <c r="DR3" t="inlineStr"/>
+      <c r="DS3" t="inlineStr"/>
+      <c r="DT3" t="inlineStr"/>
+      <c r="DU3" t="inlineStr"/>
+      <c r="DV3" t="inlineStr"/>
+      <c r="DW3" t="inlineStr"/>
+      <c r="DX3" t="inlineStr"/>
+      <c r="DY3" t="inlineStr"/>
+      <c r="DZ3" t="inlineStr"/>
+      <c r="EA3" t="inlineStr"/>
+      <c r="EB3" t="inlineStr"/>
+      <c r="EC3" t="inlineStr"/>
+      <c r="ED3" t="inlineStr"/>
+      <c r="EE3" t="inlineStr"/>
+      <c r="EF3" t="inlineStr"/>
+      <c r="EG3" t="inlineStr"/>
+      <c r="EH3" t="inlineStr"/>
+      <c r="EI3" t="inlineStr"/>
+      <c r="EJ3" t="inlineStr"/>
+      <c r="EK3" t="inlineStr"/>
+      <c r="EL3" t="inlineStr"/>
+      <c r="EM3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>市立將軍國小114693</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>吳潔欣</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>X</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr"/>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="inlineStr"/>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
+      <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
+      <c r="BW4" t="inlineStr"/>
+      <c r="BX4" t="inlineStr"/>
+      <c r="BY4" t="inlineStr"/>
+      <c r="BZ4" t="inlineStr"/>
+      <c r="CA4" t="inlineStr"/>
+      <c r="CB4" t="inlineStr"/>
+      <c r="CC4" t="inlineStr"/>
+      <c r="CD4" t="inlineStr"/>
+      <c r="CE4" t="inlineStr"/>
+      <c r="CF4" t="inlineStr"/>
+      <c r="CG4" t="inlineStr"/>
+      <c r="CH4" t="inlineStr"/>
+      <c r="CI4" t="inlineStr"/>
+      <c r="CJ4" t="inlineStr"/>
+      <c r="CK4" t="inlineStr"/>
+      <c r="CL4" t="inlineStr"/>
+      <c r="CM4" t="inlineStr"/>
+      <c r="CN4" t="inlineStr"/>
+      <c r="CO4" t="inlineStr"/>
+      <c r="CP4" t="inlineStr"/>
+      <c r="CQ4" t="inlineStr"/>
+      <c r="CR4" t="inlineStr"/>
+      <c r="CS4" t="inlineStr"/>
+      <c r="CT4" t="inlineStr"/>
+      <c r="CU4" t="inlineStr"/>
+      <c r="CV4" t="inlineStr"/>
+      <c r="CW4" t="inlineStr"/>
+      <c r="CX4" t="inlineStr"/>
+      <c r="CY4" t="inlineStr"/>
+      <c r="CZ4" t="inlineStr"/>
+      <c r="DA4" t="inlineStr"/>
+      <c r="DB4" t="inlineStr"/>
+      <c r="DC4" t="inlineStr"/>
+      <c r="DD4" t="inlineStr"/>
+      <c r="DE4" t="inlineStr"/>
+      <c r="DF4" t="inlineStr"/>
+      <c r="DG4" t="inlineStr"/>
+      <c r="DH4" t="inlineStr"/>
+      <c r="DI4" t="inlineStr"/>
+      <c r="DJ4" t="inlineStr"/>
+      <c r="DK4" t="inlineStr"/>
+      <c r="DL4" t="inlineStr"/>
+      <c r="DM4" t="inlineStr"/>
+      <c r="DN4" t="inlineStr"/>
+      <c r="DO4" t="inlineStr"/>
+      <c r="DP4" t="inlineStr"/>
+      <c r="DQ4" t="inlineStr"/>
+      <c r="DR4" t="inlineStr"/>
+      <c r="DS4" t="inlineStr"/>
+      <c r="DT4" t="inlineStr"/>
+      <c r="DU4" t="inlineStr"/>
+      <c r="DV4" t="inlineStr"/>
+      <c r="DW4" t="inlineStr"/>
+      <c r="DX4" t="inlineStr"/>
+      <c r="DY4" t="inlineStr"/>
+      <c r="DZ4" t="inlineStr"/>
+      <c r="EA4" t="inlineStr"/>
+      <c r="EB4" t="inlineStr"/>
+      <c r="EC4" t="inlineStr"/>
+      <c r="ED4" t="inlineStr"/>
+      <c r="EE4" t="inlineStr"/>
+      <c r="EF4" t="inlineStr"/>
+      <c r="EG4" t="inlineStr"/>
+      <c r="EH4" t="inlineStr"/>
+      <c r="EI4" t="inlineStr"/>
+      <c r="EJ4" t="inlineStr"/>
+      <c r="EK4" t="inlineStr"/>
+      <c r="EL4" t="inlineStr"/>
+      <c r="EM4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>市立將軍國小114693</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>陳彥汝</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr"/>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr"/>
+      <c r="AA5" t="inlineStr"/>
+      <c r="AB5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr"/>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
+      <c r="AR5" t="inlineStr"/>
+      <c r="AS5" t="inlineStr"/>
+      <c r="AT5" t="inlineStr"/>
+      <c r="AU5" t="inlineStr"/>
+      <c r="AV5" t="inlineStr"/>
+      <c r="AW5" t="inlineStr"/>
+      <c r="AX5" t="inlineStr"/>
+      <c r="AY5" t="inlineStr"/>
+      <c r="AZ5" t="inlineStr"/>
+      <c r="BA5" t="inlineStr"/>
+      <c r="BB5" t="inlineStr"/>
+      <c r="BC5" t="inlineStr"/>
+      <c r="BD5" t="inlineStr"/>
+      <c r="BE5" t="inlineStr"/>
+      <c r="BF5" t="inlineStr"/>
+      <c r="BG5" t="inlineStr"/>
+      <c r="BH5" t="inlineStr"/>
+      <c r="BI5" t="inlineStr"/>
+      <c r="BJ5" t="inlineStr"/>
+      <c r="BK5" t="inlineStr"/>
+      <c r="BL5" t="inlineStr"/>
+      <c r="BM5" t="inlineStr"/>
+      <c r="BN5" t="inlineStr"/>
+      <c r="BO5" t="inlineStr"/>
+      <c r="BP5" t="inlineStr"/>
+      <c r="BQ5" t="inlineStr"/>
+      <c r="BR5" t="inlineStr"/>
+      <c r="BS5" t="inlineStr"/>
+      <c r="BT5" t="inlineStr"/>
+      <c r="BU5" t="inlineStr"/>
+      <c r="BV5" t="inlineStr"/>
+      <c r="BW5" t="inlineStr"/>
+      <c r="BX5" t="inlineStr"/>
+      <c r="BY5" t="inlineStr"/>
+      <c r="BZ5" t="inlineStr"/>
+      <c r="CA5" t="inlineStr"/>
+      <c r="CB5" t="inlineStr"/>
+      <c r="CC5" t="inlineStr"/>
+      <c r="CD5" t="inlineStr"/>
+      <c r="CE5" t="inlineStr"/>
+      <c r="CF5" t="inlineStr"/>
+      <c r="CG5" t="inlineStr"/>
+      <c r="CH5" t="inlineStr"/>
+      <c r="CI5" t="inlineStr"/>
+      <c r="CJ5" t="inlineStr"/>
+      <c r="CK5" t="inlineStr"/>
+      <c r="CL5" t="inlineStr"/>
+      <c r="CM5" t="inlineStr"/>
+      <c r="CN5" t="inlineStr"/>
+      <c r="CO5" t="inlineStr"/>
+      <c r="CP5" t="inlineStr"/>
+      <c r="CQ5" t="inlineStr"/>
+      <c r="CR5" t="inlineStr"/>
+      <c r="CS5" t="inlineStr"/>
+      <c r="CT5" t="inlineStr"/>
+      <c r="CU5" t="inlineStr"/>
+      <c r="CV5" t="inlineStr"/>
+      <c r="CW5" t="inlineStr"/>
+      <c r="CX5" t="inlineStr"/>
+      <c r="CY5" t="inlineStr"/>
+      <c r="CZ5" t="inlineStr"/>
+      <c r="DA5" t="inlineStr"/>
+      <c r="DB5" t="inlineStr"/>
+      <c r="DC5" t="inlineStr"/>
+      <c r="DD5" t="inlineStr"/>
+      <c r="DE5" t="inlineStr"/>
+      <c r="DF5" t="inlineStr"/>
+      <c r="DG5" t="inlineStr"/>
+      <c r="DH5" t="inlineStr"/>
+      <c r="DI5" t="inlineStr"/>
+      <c r="DJ5" t="inlineStr"/>
+      <c r="DK5" t="inlineStr"/>
+      <c r="DL5" t="inlineStr"/>
+      <c r="DM5" t="inlineStr"/>
+      <c r="DN5" t="inlineStr"/>
+      <c r="DO5" t="inlineStr"/>
+      <c r="DP5" t="inlineStr"/>
+      <c r="DQ5" t="inlineStr"/>
+      <c r="DR5" t="inlineStr"/>
+      <c r="DS5" t="inlineStr"/>
+      <c r="DT5" t="inlineStr"/>
+      <c r="DU5" t="inlineStr"/>
+      <c r="DV5" t="inlineStr"/>
+      <c r="DW5" t="inlineStr"/>
+      <c r="DX5" t="inlineStr"/>
+      <c r="DY5" t="inlineStr"/>
+      <c r="DZ5" t="inlineStr"/>
+      <c r="EA5" t="inlineStr"/>
+      <c r="EB5" t="inlineStr"/>
+      <c r="EC5" t="inlineStr"/>
+      <c r="ED5" t="inlineStr"/>
+      <c r="EE5" t="inlineStr"/>
+      <c r="EF5" t="inlineStr"/>
+      <c r="EG5" t="inlineStr"/>
+      <c r="EH5" t="inlineStr"/>
+      <c r="EI5" t="inlineStr"/>
+      <c r="EJ5" t="inlineStr"/>
+      <c r="EK5" t="inlineStr"/>
+      <c r="EL5" t="inlineStr"/>
+      <c r="EM5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>